<commit_message>
swap prediction males females
</commit_message>
<xml_diff>
--- a/media/predictions/3.xlsx
+++ b/media/predictions/3.xlsx
@@ -16,9 +16,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="42">
-  <si>
-    <t>Заплив №1 - Чоловіки</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="41">
+  <si>
+    <t>Заплив №1 - Жінки</t>
   </si>
   <si>
     <t>Дистанція №1 - 100 Вільний стиль</t>
@@ -42,15 +42,27 @@
     <t>Доріжка</t>
   </si>
   <si>
+    <t>6 6</t>
+  </si>
+  <si>
+    <t>A(25-29)</t>
+  </si>
+  <si>
+    <t>Single</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>Заплив №2 - Чоловіки</t>
+  </si>
+  <si>
     <t>admin admin</t>
   </si>
   <si>
     <t>None(None)</t>
   </si>
   <si>
-    <t>Single</t>
-  </si>
-  <si>
     <t>dsad</t>
   </si>
   <si>
@@ -84,7 +96,7 @@
     <t>2</t>
   </si>
   <si>
-    <t>Заплив №2 - Чоловіки</t>
+    <t>Заплив №3 - Чоловіки</t>
   </si>
   <si>
     <t>авы авы</t>
@@ -93,55 +105,40 @@
     <t>авы</t>
   </si>
   <si>
+    <t>Заплив №4 - Жінки</t>
+  </si>
+  <si>
+    <t>Дистанція №2 - 50 Брас</t>
+  </si>
+  <si>
+    <t>Заплив №5 - Чоловіки</t>
+  </si>
+  <si>
+    <t>Заплив №6 - Жінки</t>
+  </si>
+  <si>
+    <t>Дистанція №3 - 100 Баттерфлай</t>
+  </si>
+  <si>
+    <t>Заплив №7 - Чоловіки</t>
+  </si>
+  <si>
+    <t>Заплив №8 - Жінки</t>
+  </si>
+  <si>
+    <t>Дистанція №4 - 100 Комплексне плавання</t>
+  </si>
+  <si>
+    <t>Заплив №9 - Чоловіки</t>
+  </si>
+  <si>
     <t>Заплив №3 - Жінки</t>
   </si>
   <si>
-    <t>6 6</t>
-  </si>
-  <si>
-    <t>A(25-29)</t>
-  </si>
-  <si>
-    <t>6</t>
+    <t>Дистанція №2 - 50 Вільний стиль</t>
   </si>
   <si>
     <t>Заплив №4 - Чоловіки</t>
-  </si>
-  <si>
-    <t>Дистанція №2 - 50 Брас</t>
-  </si>
-  <si>
-    <t>Заплив №5 - Жінки</t>
-  </si>
-  <si>
-    <t>Заплив №6 - Чоловіки</t>
-  </si>
-  <si>
-    <t>Дистанція №3 - 100 Баттерфлай</t>
-  </si>
-  <si>
-    <t>Заплив №7 - Жінки</t>
-  </si>
-  <si>
-    <t>Заплив №8 - Чоловіки</t>
-  </si>
-  <si>
-    <t>Дистанція №4 - 100 Комплексне плавання</t>
-  </si>
-  <si>
-    <t>Заплив №9 - Жінки</t>
-  </si>
-  <si>
-    <t>Заплив №2 - Жінки</t>
-  </si>
-  <si>
-    <t>Заплив №3 - Чоловіки</t>
-  </si>
-  <si>
-    <t>Дистанція №2 - 50 Вільний стиль</t>
-  </si>
-  <si>
-    <t>Заплив №4 - Жінки</t>
   </si>
 </sst>
 </file>
@@ -511,7 +508,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F86"/>
+  <dimension ref="A1:F89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -572,75 +569,15 @@
         <v>11</v>
       </c>
       <c r="E6" s="5" t="n">
-        <v>0.466099537037037</v>
+        <v>0.0003819444444444445</v>
       </c>
       <c r="F6" s="4" t="n">
         <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="5" t="n">
-        <v>0.0005092592592592592</v>
-      </c>
-      <c r="F7" s="4" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" s="5" t="n">
-        <v>0.0006134259259259259</v>
-      </c>
-      <c r="F8" s="4" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="5" t="n">
-        <v>0.0006365740740740741</v>
-      </c>
-      <c r="F9" s="4" t="n">
-        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -673,27 +610,87 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" s="5" t="n">
+        <v>0.466099537037037</v>
+      </c>
+      <c r="F16" s="4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="5" t="n">
+        <v>0.0005092592592592592</v>
+      </c>
+      <c r="F17" s="4" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" s="5" t="n">
+        <v>0.0006134259259259259</v>
+      </c>
+      <c r="F18" s="4" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16" s="4" t="s">
+      <c r="B19" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E16" s="5" t="n">
-        <v>0.0003819444444444445</v>
-      </c>
-      <c r="F16" s="4" t="n">
-        <v>1</v>
+      <c r="C19" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19" s="5" t="n">
+        <v>0.0006365740740740741</v>
+      </c>
+      <c r="F19" s="4" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -726,13 +723,13 @@
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>28</v>
@@ -779,82 +776,22 @@
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="4" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E36" s="5" t="n">
-        <v>0.0004976851851851852</v>
+        <v>0.0003819444444444445</v>
       </c>
       <c r="F36" s="4" t="n">
         <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="A37" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E37" s="5" t="n">
-        <v>0.0002662037037037037</v>
-      </c>
-      <c r="F37" s="4" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
-      <c r="A38" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E38" s="5" t="n">
-        <v>0.0003819444444444445</v>
-      </c>
-      <c r="F38" s="4" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
-      <c r="A39" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E39" s="5" t="n">
-        <v>0.0003819444444444445</v>
-      </c>
-      <c r="F39" s="4" t="n">
-        <v>4</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -892,22 +829,82 @@
     </row>
     <row r="46" spans="1:6">
       <c r="A46" s="4" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B46" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E46" s="5" t="n">
+        <v>0.0004976851851851852</v>
+      </c>
+      <c r="F46" s="4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E47" s="5" t="n">
+        <v>0.0002662037037037037</v>
+      </c>
+      <c r="F47" s="4" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E48" s="5" t="n">
+        <v>0.0003819444444444445</v>
+      </c>
+      <c r="F48" s="4" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C46" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D46" s="4" t="s">
+      <c r="B49" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D49" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E46" s="5" t="n">
+      <c r="E49" s="5" t="n">
         <v>0.0003819444444444445</v>
       </c>
-      <c r="F46" s="4" t="n">
-        <v>1</v>
+      <c r="F49" s="4" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -945,82 +942,22 @@
     </row>
     <row r="56" spans="1:6">
       <c r="A56" s="4" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="E56" s="5" t="n">
-        <v>0.0005092592592592592</v>
+        <v>0.0002546296296296296</v>
       </c>
       <c r="F56" s="4" t="n">
         <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6">
-      <c r="A57" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B57" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D57" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E57" s="5" t="n">
-        <v>0.0002546296296296296</v>
-      </c>
-      <c r="F57" s="4" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6">
-      <c r="A58" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B58" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C58" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D58" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E58" s="5" t="n">
-        <v>0.0002662037037037037</v>
-      </c>
-      <c r="F58" s="4" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6">
-      <c r="A59" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B59" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D59" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E59" s="5" t="n">
-        <v>0.0003703703703703704</v>
-      </c>
-      <c r="F59" s="4" t="n">
-        <v>4</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -1058,22 +995,82 @@
     </row>
     <row r="66" spans="1:6">
       <c r="A66" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="D66" s="4" t="s">
         <v>28</v>
       </c>
       <c r="E66" s="5" t="n">
+        <v>0.0005092592592592592</v>
+      </c>
+      <c r="F66" s="4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6">
+      <c r="A67" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D67" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E67" s="5" t="n">
         <v>0.0002546296296296296</v>
       </c>
-      <c r="F66" s="4" t="n">
-        <v>1</v>
+      <c r="F67" s="4" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
+      <c r="A68" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D68" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E68" s="5" t="n">
+        <v>0.0002662037037037037</v>
+      </c>
+      <c r="F68" s="4" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6">
+      <c r="A69" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E69" s="5" t="n">
+        <v>0.0003703703703703704</v>
+      </c>
+      <c r="F69" s="4" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -1111,82 +1108,22 @@
     </row>
     <row r="76" spans="1:6">
       <c r="A76" s="4" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E76" s="5" t="n">
-        <v>0.0005092592592592592</v>
+        <v>0.0004976851851851852</v>
       </c>
       <c r="F76" s="4" t="n">
         <v>1</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6">
-      <c r="A77" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B77" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C77" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D77" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E77" s="5" t="n">
-        <v>0.0001273148148148148</v>
-      </c>
-      <c r="F77" s="4" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6">
-      <c r="A78" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B78" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C78" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D78" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E78" s="5" t="n">
-        <v>0.000162037037037037</v>
-      </c>
-      <c r="F78" s="4" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6">
-      <c r="A79" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B79" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C79" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D79" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E79" s="5" t="n">
-        <v>0.0002546296296296296</v>
-      </c>
-      <c r="F79" s="4" t="n">
-        <v>4</v>
       </c>
     </row>
     <row r="81" spans="1:6">
@@ -1224,22 +1161,82 @@
     </row>
     <row r="86" spans="1:6">
       <c r="A86" s="4" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B86" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C86" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D86" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E86" s="5" t="n">
+        <v>0.0005092592592592592</v>
+      </c>
+      <c r="F86" s="4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6">
+      <c r="A87" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B87" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C87" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D87" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E87" s="5" t="n">
+        <v>0.0001273148148148148</v>
+      </c>
+      <c r="F87" s="4" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6">
+      <c r="A88" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B88" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C88" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D88" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E88" s="5" t="n">
+        <v>0.000162037037037037</v>
+      </c>
+      <c r="F88" s="4" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6">
+      <c r="A89" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C86" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D86" s="4" t="s">
+      <c r="B89" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C89" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D89" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E86" s="5" t="n">
-        <v>0.0004976851851851852</v>
-      </c>
-      <c r="F86" s="4" t="n">
-        <v>1</v>
+      <c r="E89" s="5" t="n">
+        <v>0.0002546296296296296</v>
+      </c>
+      <c r="F89" s="4" t="n">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -1282,7 +1279,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1331,87 +1328,27 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="4" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="E6" s="5" t="n">
-        <v>0.000625</v>
+        <v>0.0006828703703703704</v>
       </c>
       <c r="F6" s="4" t="n">
         <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="5" t="n">
-        <v>0.0002662037037037037</v>
-      </c>
-      <c r="F7" s="4" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" s="5" t="n">
-        <v>0.0004976851851851852</v>
-      </c>
-      <c r="F8" s="4" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" s="5" t="n">
-        <v>0.0005092592592592592</v>
-      </c>
-      <c r="F9" s="4" t="n">
-        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1444,32 +1381,92 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>28</v>
       </c>
       <c r="E16" s="5" t="n">
-        <v>0.0006828703703703704</v>
+        <v>0.000625</v>
       </c>
       <c r="F16" s="4" t="n">
         <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="5" t="n">
+        <v>0.0002662037037037037</v>
+      </c>
+      <c r="F17" s="4" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" s="5" t="n">
+        <v>0.0004976851851851852</v>
+      </c>
+      <c r="F18" s="4" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" s="5" t="n">
+        <v>0.0005092592592592592</v>
+      </c>
+      <c r="F19" s="4" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1497,92 +1494,32 @@
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="4" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="E26" s="5" t="n">
-        <v>0.0006365740740740741</v>
+        <v>0.0005092592592592592</v>
       </c>
       <c r="F26" s="4" t="n">
         <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E27" s="5" t="n">
-        <v>0.0003703703703703704</v>
-      </c>
-      <c r="F27" s="4" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E28" s="5" t="n">
-        <v>0.0003935185185185185</v>
-      </c>
-      <c r="F28" s="4" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E29" s="5" t="n">
-        <v>0.0003935185185185185</v>
-      </c>
-      <c r="F29" s="4" t="n">
-        <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1610,22 +1547,82 @@
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="D36" s="4" t="s">
         <v>28</v>
       </c>
       <c r="E36" s="5" t="n">
-        <v>0.0005092592592592592</v>
+        <v>0.0006365740740740741</v>
       </c>
       <c r="F36" s="4" t="n">
         <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E37" s="5" t="n">
+        <v>0.0003703703703703704</v>
+      </c>
+      <c r="F37" s="4" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E38" s="5" t="n">
+        <v>0.0003935185185185185</v>
+      </c>
+      <c r="F38" s="4" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E39" s="5" t="n">
+        <v>0.0003935185185185185</v>
+      </c>
+      <c r="F39" s="4" t="n">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
a lot of shit was added
</commit_message>
<xml_diff>
--- a/media/predictions/3.xlsx
+++ b/media/predictions/3.xlsx
@@ -7,8 +7,8 @@
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="День 1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="День 2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Day 1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Day 2" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -18,28 +18,28 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="41">
   <si>
-    <t>Заплив №1 - Жінки</t>
-  </si>
-  <si>
-    <t>Дистанція №1 - 100 Вільний стиль</t>
-  </si>
-  <si>
-    <t>Учасник</t>
-  </si>
-  <si>
-    <t>Вікова група</t>
-  </si>
-  <si>
-    <t>Команда</t>
-  </si>
-  <si>
-    <t>Місто</t>
-  </si>
-  <si>
-    <t>Час</t>
-  </si>
-  <si>
-    <t>Доріжка</t>
+    <t>Swim №1 - Females</t>
+  </si>
+  <si>
+    <t>Distance №1 - 100 Freestyle</t>
+  </si>
+  <si>
+    <t>Member</t>
+  </si>
+  <si>
+    <t>Age group</t>
+  </si>
+  <si>
+    <t>Team</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Track</t>
   </si>
   <si>
     <t>6 6</t>
@@ -54,7 +54,7 @@
     <t>6</t>
   </si>
   <si>
-    <t>Заплив №2 - Чоловіки</t>
+    <t>Swim №2 - Males</t>
   </si>
   <si>
     <t>admin admin</t>
@@ -96,7 +96,7 @@
     <t>2</t>
   </si>
   <si>
-    <t>Заплив №3 - Чоловіки</t>
+    <t>Swim №3 - Males</t>
   </si>
   <si>
     <t>Жабран Ильйа</t>
@@ -105,40 +105,40 @@
     <t>авы</t>
   </si>
   <si>
-    <t>Заплив №4 - Жінки</t>
-  </si>
-  <si>
-    <t>Дистанція №2 - 50 Брас</t>
-  </si>
-  <si>
-    <t>Заплив №5 - Чоловіки</t>
-  </si>
-  <si>
-    <t>Заплив №6 - Жінки</t>
-  </si>
-  <si>
-    <t>Дистанція №3 - 100 Баттерфлай</t>
-  </si>
-  <si>
-    <t>Заплив №7 - Чоловіки</t>
-  </si>
-  <si>
-    <t>Заплив №8 - Жінки</t>
-  </si>
-  <si>
-    <t>Дистанція №4 - 100 Комплексне плавання</t>
-  </si>
-  <si>
-    <t>Заплив №9 - Чоловіки</t>
-  </si>
-  <si>
-    <t>Заплив №3 - Жінки</t>
-  </si>
-  <si>
-    <t>Дистанція №2 - 50 Вільний стиль</t>
-  </si>
-  <si>
-    <t>Заплив №4 - Чоловіки</t>
+    <t>Swim №4 - Females</t>
+  </si>
+  <si>
+    <t>Distance №2 - 50 Breaststroke</t>
+  </si>
+  <si>
+    <t>Swim №5 - Males</t>
+  </si>
+  <si>
+    <t>Swim №6 - Females</t>
+  </si>
+  <si>
+    <t>Distance №3 - 100 Butterfly</t>
+  </si>
+  <si>
+    <t>Swim №7 - Males</t>
+  </si>
+  <si>
+    <t>Swim №8 - Females</t>
+  </si>
+  <si>
+    <t>Distance №4 - 100 Dolphin kick</t>
+  </si>
+  <si>
+    <t>Swim №9 - Males</t>
+  </si>
+  <si>
+    <t>Swim №3 - Females</t>
+  </si>
+  <si>
+    <t>Distance №2 - 50 Freestyle</t>
+  </si>
+  <si>
+    <t>Swim №4 - Males</t>
   </si>
 </sst>
 </file>

</xml_diff>